<commit_message>
Add split between deep and shallow networks with some initial setup
</commit_message>
<xml_diff>
--- a/doc/final_project_experiments.xlsx
+++ b/doc/final_project_experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hurtja/Documents/Spring2018/CI/CNNFinalProject/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844C5478-B06A-5C4F-A92B-D008BA338B3B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505D76AD-0141-6C4B-AAE8-9DAC299C79C1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10980" yWindow="440" windowWidth="22620" windowHeight="19480" xr2:uid="{F6E77F36-42F3-3D4F-B027-6FE579A9FCA2}"/>
   </bookViews>
@@ -499,7 +499,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -830,7 +830,9 @@
       <c r="H11" s="1">
         <v>120</v>
       </c>
-      <c r="I11" s="1"/>
+      <c r="I11" s="1">
+        <v>0.618319801057855</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bring things into Util
</commit_message>
<xml_diff>
--- a/doc/final_project_experiments.xlsx
+++ b/doc/final_project_experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hurtja/Documents/Spring2018/CI/CNNFinalProject/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505D76AD-0141-6C4B-AAE8-9DAC299C79C1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898F45D3-CB5C-6347-85C2-05EB012B51FA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10980" yWindow="440" windowWidth="22620" windowHeight="19480" xr2:uid="{F6E77F36-42F3-3D4F-B027-6FE579A9FCA2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>Folds</t>
   </si>
@@ -182,8 +182,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EC684B55-4795-B049-A98F-0A28F08D170D}" name="Table1" displayName="Table1" ref="A1:I11" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="A1:I11" xr:uid="{29C0021A-7284-4F4D-92CC-F4FB504F51EB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EC684B55-4795-B049-A98F-0A28F08D170D}" name="Table1" displayName="Table1" ref="A1:I12" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A1:I12" xr:uid="{29C0021A-7284-4F4D-92CC-F4FB504F51EB}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{E1CA67D2-2BB9-7A44-BCDF-DBD484E70FF8}" name="Dataset" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{377F0843-4415-E443-B633-33B51083B561}" name="Desciption" dataCellStyle="Normal"/>
@@ -496,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C7FFB1-92F7-C642-8DB7-9D32F33F3A3D}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -834,6 +834,35 @@
         <v>0.618319801057855</v>
       </c>
     </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>5</v>
+      </c>
+      <c r="H12" s="1">
+        <v>300</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.60240090983541095</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Add new experiment and use command line params
</commit_message>
<xml_diff>
--- a/doc/final_project_experiments.xlsx
+++ b/doc/final_project_experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hurtja/Documents/Spring2018/CI/CNNFinalProject/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898F45D3-CB5C-6347-85C2-05EB012B51FA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A83FE8-35AE-5C48-A15D-1809F3231D9B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10980" yWindow="440" windowWidth="22620" windowHeight="19480" xr2:uid="{F6E77F36-42F3-3D4F-B027-6FE579A9FCA2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
   <si>
     <t>Folds</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t>More Layers &amp; More Epochs</t>
+  </si>
+  <si>
+    <t>Shallow Experiments</t>
+  </si>
+  <si>
+    <t>DCNN Experiments</t>
+  </si>
+  <si>
+    <t>DRNN Experiments</t>
+  </si>
+  <si>
+    <t>Extra Epochs</t>
   </si>
 </sst>
 </file>
@@ -108,7 +120,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -116,18 +128,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -182,18 +261,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EC684B55-4795-B049-A98F-0A28F08D170D}" name="Table1" displayName="Table1" ref="A1:I12" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="A1:I12" xr:uid="{29C0021A-7284-4F4D-92CC-F4FB504F51EB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EC684B55-4795-B049-A98F-0A28F08D170D}" name="Table1" displayName="Table1" ref="A2:I13" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A2:I13" xr:uid="{29C0021A-7284-4F4D-92CC-F4FB504F51EB}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{E1CA67D2-2BB9-7A44-BCDF-DBD484E70FF8}" name="Dataset" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{377F0843-4415-E443-B633-33B51083B561}" name="Desciption" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{A9A336A6-A34E-764A-AC78-B135B81CA9DB}" name="Folds" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{09DCAD2A-2E57-A44A-956C-B0244C604FE4}" name="Filters" dataDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{7AE1DAE2-E815-C447-AC85-D5EE10F536C1}" name="Kernel Size" dataDxfId="2" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{7E564357-F8B8-C540-80C0-52BF9A6692C0}" name="Pooling Size" dataDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{1A26F601-654D-C748-8B27-0F44BF1E3E1D}" name="Layers" dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{A9A336A6-A34E-764A-AC78-B135B81CA9DB}" name="Folds" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{09DCAD2A-2E57-A44A-956C-B0244C604FE4}" name="Filters" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{7AE1DAE2-E815-C447-AC85-D5EE10F536C1}" name="Kernel Size" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{7E564357-F8B8-C540-80C0-52BF9A6692C0}" name="Pooling Size" dataDxfId="7" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{1A26F601-654D-C748-8B27-0F44BF1E3E1D}" name="Layers" dataDxfId="6" dataCellStyle="Normal"/>
     <tableColumn id="7" xr3:uid="{4B95C30D-C2F2-9444-B84A-C0AB21566CD7}" name="Epochs" dataCellStyle="Normal"/>
     <tableColumn id="8" xr3:uid="{B18F30EC-B0E0-5642-BA88-12994A2B1358}" name="Avg Accuracy" dataCellStyle="Normal"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2ECF387E-6482-B644-9FDF-9712C56D7E74}" name="Table13" displayName="Table13" ref="A16:E18" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A16:E18" xr:uid="{4A1B07B0-B6C5-4C48-A6FF-1D5F73836EF5}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{C34DCD86-FE6B-9347-9458-3A49D92D1494}" name="Dataset" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{1FEC8DF8-6D02-3C41-9C03-3C4A8E4CB895}" name="Desciption" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{E4E323CA-5EC0-0547-96EC-26DEE56EA39E}" name="Folds" dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{DBA63CFB-F2DC-6145-8C11-1351E0588060}" name="Epochs" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{82785D70-20CD-AA4C-A4F4-246F1CFE5C91}" name="Avg Accuracy" dataDxfId="3" dataCellStyle="Normal"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EF1F4B09-EB2C-B640-8DCF-96624F09A3F2}" name="Table134" displayName="Table134" ref="A21:E22" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A21:E22" xr:uid="{2CD76283-3A3D-CD4B-948F-0F24B7AC75CA}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{B7A3EE2A-5771-E744-996D-229D7B1BF495}" name="Dataset" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{273A97CF-35D6-DB47-9ED0-488F01CB85D0}" name="Desciption" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{03F3BD62-F46F-414C-B27E-F31F0C0DAE16}" name="Folds" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{B477439E-272F-7647-824C-F921B6B099CB}" name="Epochs" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{90650614-8CAF-C848-A9C7-1AB4E4E9AD62}" name="Avg Accuracy" dataDxfId="0" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -496,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C7FFB1-92F7-C642-8DB7-9D32F33F3A3D}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,7 +615,7 @@
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -516,69 +623,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="1">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1">
-        <v>32</v>
-      </c>
-      <c r="E2" s="1">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>10</v>
-      </c>
-      <c r="I2">
-        <v>0.91167153589957195</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>5</v>
@@ -596,18 +687,18 @@
         <v>2</v>
       </c>
       <c r="H3">
-        <v>20</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0.93149619414609897</v>
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>0.91167153589957195</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
         <v>5</v>
@@ -625,10 +716,10 @@
         <v>2</v>
       </c>
       <c r="H4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I4" s="1">
-        <v>0.52214192616261002</v>
+        <v>0.93149619414609897</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -636,7 +727,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1">
         <v>5</v>
@@ -653,11 +744,11 @@
       <c r="G5" s="1">
         <v>2</v>
       </c>
-      <c r="H5" s="1">
-        <v>50</v>
+      <c r="H5">
+        <v>10</v>
       </c>
       <c r="I5" s="1">
-        <v>0.53902418348453895</v>
+        <v>0.52214192616261002</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -665,7 +756,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
@@ -683,10 +774,10 @@
         <v>2</v>
       </c>
       <c r="H6" s="1">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="I6" s="1">
-        <v>0.5402862469545</v>
+        <v>0.53902418348453895</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -694,7 +785,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1">
         <v>5</v>
@@ -709,13 +800,13 @@
         <v>2</v>
       </c>
       <c r="G7" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H7" s="1">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="I7" s="1">
-        <v>0.59042631709990001</v>
+        <v>0.5402862469545</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -723,7 +814,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1">
         <v>5</v>
@@ -738,13 +829,13 @@
         <v>2</v>
       </c>
       <c r="G8" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H8" s="1">
-        <v>500</v>
+        <v>25</v>
       </c>
       <c r="I8" s="1">
-        <v>0.14965451869100899</v>
+        <v>0.59042631709990001</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -752,7 +843,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1">
         <v>5</v>
@@ -770,10 +861,10 @@
         <v>6</v>
       </c>
       <c r="H9" s="1">
-        <v>120</v>
+        <v>500</v>
       </c>
       <c r="I9" s="1">
-        <v>0.57629963003837203</v>
+        <v>0.14965451869100899</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -781,7 +872,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1">
         <v>5</v>
@@ -796,13 +887,13 @@
         <v>2</v>
       </c>
       <c r="G10" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H10" s="1">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="I10" s="1">
-        <v>0.60594214650054301</v>
+        <v>0.57629963003837203</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -828,10 +919,10 @@
         <v>5</v>
       </c>
       <c r="H11" s="1">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="I11" s="1">
-        <v>0.618319801057855</v>
+        <v>0.60594214650054301</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -857,16 +948,245 @@
         <v>5</v>
       </c>
       <c r="H12" s="1">
+        <v>120</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.618319801057855</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1">
+        <v>32</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>5</v>
+      </c>
+      <c r="H13" s="1">
         <v>300</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I13" s="1">
         <v>0.60240090983541095</v>
       </c>
     </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>0.75528930555234297</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1">
+        <v>50</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
+      </c>
+      <c r="E22">
+        <v>0.65935125244040005</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A20:E20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add more to results of experiments doc
</commit_message>
<xml_diff>
--- a/doc/final_project_experiments.xlsx
+++ b/doc/final_project_experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hurtja/Documents/Spring2018/CI/CNNFinalProject/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A83FE8-35AE-5C48-A15D-1809F3231D9B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A41425-C280-374B-957A-88BF92705FF5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10980" yWindow="440" windowWidth="22620" windowHeight="19480" xr2:uid="{F6E77F36-42F3-3D4F-B027-6FE579A9FCA2}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19520" xr2:uid="{F6E77F36-42F3-3D4F-B027-6FE579A9FCA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
   <si>
     <t>Folds</t>
   </si>
@@ -97,13 +97,19 @@
   </si>
   <si>
     <t>Extra Epochs</t>
+  </si>
+  <si>
+    <t>Batch Size: 32</t>
+  </si>
+  <si>
+    <t>Batch Size: 16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,16 +117,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -143,46 +161,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -266,11 +285,11 @@
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{E1CA67D2-2BB9-7A44-BCDF-DBD484E70FF8}" name="Dataset" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{377F0843-4415-E443-B633-33B51083B561}" name="Desciption" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{A9A336A6-A34E-764A-AC78-B135B81CA9DB}" name="Folds" dataDxfId="10" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{09DCAD2A-2E57-A44A-956C-B0244C604FE4}" name="Filters" dataDxfId="9" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{7AE1DAE2-E815-C447-AC85-D5EE10F536C1}" name="Kernel Size" dataDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{7E564357-F8B8-C540-80C0-52BF9A6692C0}" name="Pooling Size" dataDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{1A26F601-654D-C748-8B27-0F44BF1E3E1D}" name="Layers" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{A9A336A6-A34E-764A-AC78-B135B81CA9DB}" name="Folds" dataDxfId="7" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{09DCAD2A-2E57-A44A-956C-B0244C604FE4}" name="Filters" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{7AE1DAE2-E815-C447-AC85-D5EE10F536C1}" name="Kernel Size" dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{7E564357-F8B8-C540-80C0-52BF9A6692C0}" name="Pooling Size" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{1A26F601-654D-C748-8B27-0F44BF1E3E1D}" name="Layers" dataDxfId="3" dataCellStyle="Normal"/>
     <tableColumn id="7" xr3:uid="{4B95C30D-C2F2-9444-B84A-C0AB21566CD7}" name="Epochs" dataCellStyle="Normal"/>
     <tableColumn id="8" xr3:uid="{B18F30EC-B0E0-5642-BA88-12994A2B1358}" name="Avg Accuracy" dataCellStyle="Normal"/>
   </tableColumns>
@@ -284,23 +303,23 @@
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{C34DCD86-FE6B-9347-9458-3A49D92D1494}" name="Dataset" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{1FEC8DF8-6D02-3C41-9C03-3C4A8E4CB895}" name="Desciption" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{E4E323CA-5EC0-0547-96EC-26DEE56EA39E}" name="Folds" dataDxfId="5" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{DBA63CFB-F2DC-6145-8C11-1351E0588060}" name="Epochs" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{82785D70-20CD-AA4C-A4F4-246F1CFE5C91}" name="Avg Accuracy" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{E4E323CA-5EC0-0547-96EC-26DEE56EA39E}" name="Folds" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{DBA63CFB-F2DC-6145-8C11-1351E0588060}" name="Epochs" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{82785D70-20CD-AA4C-A4F4-246F1CFE5C91}" name="Avg Accuracy" dataDxfId="0" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EF1F4B09-EB2C-B640-8DCF-96624F09A3F2}" name="Table134" displayName="Table134" ref="A21:E22" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EF1F4B09-EB2C-B640-8DCF-96624F09A3F2}" name="Table134" displayName="Table134" ref="A21:E22" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Good">
   <autoFilter ref="A21:E22" xr:uid="{2CD76283-3A3D-CD4B-948F-0F24B7AC75CA}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B7A3EE2A-5771-E744-996D-229D7B1BF495}" name="Dataset" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{273A97CF-35D6-DB47-9ED0-488F01CB85D0}" name="Desciption" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{03F3BD62-F46F-414C-B27E-F31F0C0DAE16}" name="Folds" dataDxfId="2" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{B477439E-272F-7647-824C-F921B6B099CB}" name="Epochs" dataDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{90650614-8CAF-C848-A9C7-1AB4E4E9AD62}" name="Avg Accuracy" dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{B7A3EE2A-5771-E744-996D-229D7B1BF495}" name="Dataset" dataCellStyle="Good"/>
+    <tableColumn id="2" xr3:uid="{273A97CF-35D6-DB47-9ED0-488F01CB85D0}" name="Desciption" dataCellStyle="Good"/>
+    <tableColumn id="3" xr3:uid="{03F3BD62-F46F-414C-B27E-F31F0C0DAE16}" name="Folds" dataCellStyle="Good"/>
+    <tableColumn id="4" xr3:uid="{B477439E-272F-7647-824C-F921B6B099CB}" name="Epochs" dataCellStyle="Good"/>
+    <tableColumn id="5" xr3:uid="{90650614-8CAF-C848-A9C7-1AB4E4E9AD62}" name="Avg Accuracy" dataCellStyle="Good"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -603,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C7FFB1-92F7-C642-8DB7-9D32F33F3A3D}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,7 +641,7 @@
     <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -635,7 +654,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -663,8 +682,11 @@
       <c r="I2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -692,37 +714,39 @@
       <c r="I3">
         <v>0.91167153589957195</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4" s="5">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5">
         <v>32</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="5">
         <v>3</v>
       </c>
-      <c r="F4" s="1">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1">
-        <v>2</v>
-      </c>
-      <c r="H4">
+      <c r="F4" s="5">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2</v>
+      </c>
+      <c r="H4" s="5">
         <v>20</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="5">
         <v>0.93149619414609897</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -750,8 +774,9 @@
       <c r="I5" s="1">
         <v>0.52214192616261002</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -779,8 +804,9 @@
       <c r="I6" s="1">
         <v>0.53902418348453895</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -808,8 +834,9 @@
       <c r="I7" s="1">
         <v>0.5402862469545</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -837,8 +864,9 @@
       <c r="I8" s="1">
         <v>0.59042631709990001</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -866,8 +894,9 @@
       <c r="I9" s="1">
         <v>0.14965451869100899</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -895,8 +924,9 @@
       <c r="I10" s="1">
         <v>0.57629963003837203</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -924,37 +954,39 @@
       <c r="I11" s="1">
         <v>0.60594214650054301</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="1">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="C12" s="5">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5">
         <v>32</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="5">
         <v>3</v>
       </c>
-      <c r="F12" s="1">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1">
-        <v>5</v>
-      </c>
-      <c r="H12" s="1">
+      <c r="F12" s="5">
+        <v>2</v>
+      </c>
+      <c r="G12" s="5">
+        <v>5</v>
+      </c>
+      <c r="H12" s="5">
         <v>120</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="5">
         <v>0.618319801057855</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -982,21 +1014,24 @@
       <c r="I13" s="1">
         <v>0.60240090983541095</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E15" s="3"/>
+      <c r="F15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1012,28 +1047,28 @@
       <c r="E16" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="7"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="1">
-        <v>5</v>
-      </c>
-      <c r="D17">
+      <c r="C17" s="5">
+        <v>5</v>
+      </c>
+      <c r="D17" s="5">
         <v>10</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="5">
         <v>0.75528930555234297</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="7"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -1052,7 +1087,7 @@
         <v>50</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="7"/>
       <c r="G18" s="1"/>
       <c r="I18" s="1"/>
     </row>
@@ -1095,28 +1130,30 @@
       <c r="E21" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="1">
-        <v>5</v>
-      </c>
-      <c r="D22">
+      <c r="C22" s="5">
+        <v>5</v>
+      </c>
+      <c r="D22" s="5">
         <v>10</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="5">
         <v>0.65935125244040005</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="F22" s="6"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -1177,10 +1214,13 @@
       <c r="I27" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="F21:F22"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="A20:E20"/>
+    <mergeCell ref="J2:J13"/>
+    <mergeCell ref="F15:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="3">

</xml_diff>

<commit_message>
Match the batch size
</commit_message>
<xml_diff>
--- a/doc/final_project_experiments.xlsx
+++ b/doc/final_project_experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hurtja/Documents/Spring2018/CI/CNNFinalProject/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A41425-C280-374B-957A-88BF92705FF5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4F5CC3-D17A-B04A-8F0C-C71C70CE3497}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19520" xr2:uid="{F6E77F36-42F3-3D4F-B027-6FE579A9FCA2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
   <si>
     <t>Folds</t>
   </si>
@@ -182,16 +182,16 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -312,8 +312,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EF1F4B09-EB2C-B640-8DCF-96624F09A3F2}" name="Table134" displayName="Table134" ref="A21:E22" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Good">
-  <autoFilter ref="A21:E22" xr:uid="{2CD76283-3A3D-CD4B-948F-0F24B7AC75CA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EF1F4B09-EB2C-B640-8DCF-96624F09A3F2}" name="Table134" displayName="Table134" ref="A21:E23" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Good">
+  <autoFilter ref="A21:E23" xr:uid="{2CD76283-3A3D-CD4B-948F-0F24B7AC75CA}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B7A3EE2A-5771-E744-996D-229D7B1BF495}" name="Dataset" dataCellStyle="Good"/>
     <tableColumn id="2" xr3:uid="{273A97CF-35D6-DB47-9ED0-488F01CB85D0}" name="Desciption" dataCellStyle="Good"/>
@@ -625,7 +625,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F21" sqref="F21:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -642,17 +642,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -717,31 +717,31 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="5">
-        <v>5</v>
-      </c>
-      <c r="D4" s="5">
+      <c r="C4" s="3">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3">
         <v>32</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>3</v>
       </c>
-      <c r="F4" s="5">
-        <v>2</v>
-      </c>
-      <c r="G4" s="5">
-        <v>2</v>
-      </c>
-      <c r="H4" s="5">
+      <c r="F4" s="3">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3">
         <v>20</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="3">
         <v>0.93149619414609897</v>
       </c>
       <c r="J4" s="7"/>
@@ -957,31 +957,31 @@
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="5">
-        <v>5</v>
-      </c>
-      <c r="D12" s="5">
+      <c r="C12" s="3">
+        <v>5</v>
+      </c>
+      <c r="D12" s="3">
         <v>32</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="3">
         <v>3</v>
       </c>
-      <c r="F12" s="5">
-        <v>2</v>
-      </c>
-      <c r="G12" s="5">
-        <v>5</v>
-      </c>
-      <c r="H12" s="5">
+      <c r="F12" s="3">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3">
+        <v>5</v>
+      </c>
+      <c r="H12" s="3">
         <v>120</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="3">
         <v>0.618319801057855</v>
       </c>
       <c r="J12" s="7"/>
@@ -1017,19 +1017,19 @@
       <c r="J13" s="7"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
       <c r="F15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1053,19 +1053,19 @@
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="A17" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="5">
-        <v>5</v>
-      </c>
-      <c r="D17" s="5">
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
         <v>10</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17">
         <v>0.75528930555234297</v>
       </c>
       <c r="F17" s="7"/>
@@ -1074,19 +1074,21 @@
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="1">
-        <v>5</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="C18" s="3">
+        <v>5</v>
+      </c>
+      <c r="D18" s="3">
         <v>50</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
       <c r="F18" s="7"/>
       <c r="G18" s="1"/>
       <c r="I18" s="1"/>
@@ -1102,13 +1104,13 @@
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1130,7 +1132,7 @@
       <c r="E21" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="4" t="s">
         <v>25</v>
       </c>
       <c r="G21" s="1"/>
@@ -1138,33 +1140,43 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="A22" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="5">
-        <v>5</v>
-      </c>
-      <c r="D22" s="5">
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
         <v>10</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22">
         <v>0.65935125244040005</v>
       </c>
-      <c r="F22" s="6"/>
+      <c r="F22" s="4"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="A23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="3">
+        <v>5</v>
+      </c>
+      <c r="D23" s="3">
+        <v>50</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.81034482853679801</v>
+      </c>
+      <c r="F23" s="4"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -1215,12 +1227,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="F21:F22"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="A20:E20"/>
     <mergeCell ref="J2:J13"/>
     <mergeCell ref="F15:F18"/>
+    <mergeCell ref="F21:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="3">

</xml_diff>

<commit_message>
Add new experiment results
</commit_message>
<xml_diff>
--- a/doc/final_project_experiments.xlsx
+++ b/doc/final_project_experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hurtja/Documents/Spring2018/CI/CNNFinalProject/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CFE1EF-57EA-B341-8047-81F845981D10}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FF755F-FAD8-6144-AFD9-D0D26AE5BB0D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="500" windowWidth="33600" windowHeight="19520" xr2:uid="{F6E77F36-42F3-3D4F-B027-6FE579A9FCA2}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="19520" xr2:uid="{F6E77F36-42F3-3D4F-B027-6FE579A9FCA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -90,10 +100,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -102,11 +113,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -136,23 +164,1253 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Test Dataset 5 Fold Cross Validation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Shallow CNN</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.91155853849810797</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.92465808979605102</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92150203932244301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89707383395541895</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.92805181678916504</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3939-6840-9F27-ECC944E22C4E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>DCNN</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.351470877777733</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33107344935587302</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33107344801990701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.57712838860485205</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.33452172584824402</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3939-6840-9F27-ECC944E22C4E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>DRNN</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.75479836118783294</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94511786517264496</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92293200531085695</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.972758618634322</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.94931034403285697</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3939-6840-9F27-ECC944E22C4E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2136663056"/>
+        <c:axId val="61471663"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2136663056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Epochs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="61471663"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="61471663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cross Validation Accuracy</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (%)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2136663056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>399143</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>34472</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>671286</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>183243</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17558B2C-F2C7-4045-8447-8B2E6DD8974D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{87B0A0FA-C3C7-2146-B266-9D906A808C95}" name="Table5" displayName="Table5" ref="A2:F5" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{87B0A0FA-C3C7-2146-B266-9D906A808C95}" name="Table5" displayName="Table5" ref="A2:F5" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A2:F5" xr:uid="{023C54D3-C4E0-0D4C-9E3C-B5C967E3EDB1}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{361F45BA-E1D9-214A-8183-6B8A0E744833}" name="Method"/>
-    <tableColumn id="2" xr3:uid="{EA2E6766-427C-2645-A26B-C347F532F8C8}" name="10"/>
-    <tableColumn id="3" xr3:uid="{A166A588-2222-8343-BC34-F16EE81825E4}" name="20"/>
-    <tableColumn id="4" xr3:uid="{ABB0FA7A-36D2-8F4D-B1BE-764E5E2B471A}" name="30"/>
-    <tableColumn id="5" xr3:uid="{B3AEFE5C-80F8-6847-9162-43DACF35AC3B}" name="40"/>
-    <tableColumn id="6" xr3:uid="{FD2CE875-7E89-324D-B301-C7FFD8CF0FE6}" name="50"/>
+    <tableColumn id="2" xr3:uid="{EA2E6766-427C-2645-A26B-C347F532F8C8}" name="10" dataDxfId="4" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{A166A588-2222-8343-BC34-F16EE81825E4}" name="20" dataDxfId="3" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{ABB0FA7A-36D2-8F4D-B1BE-764E5E2B471A}" name="30" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="5" xr3:uid="{B3AEFE5C-80F8-6847-9162-43DACF35AC3B}" name="40" dataDxfId="1" dataCellStyle="Percent"/>
+    <tableColumn id="6" xr3:uid="{FD2CE875-7E89-324D-B301-C7FFD8CF0FE6}" name="50" dataDxfId="0" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2F99A300-C080-A746-B52B-7ED60B0DC2FD}" name="Table57" displayName="Table57" ref="A8:F11" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2F99A300-C080-A746-B52B-7ED60B0DC2FD}" name="Table57" displayName="Table57" ref="A8:F11" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A8:F11" xr:uid="{0F996CB4-D350-E044-8C03-18674C1CD481}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B8882C41-F743-544E-A47C-3E26F80E0EA2}" name="Method"/>
@@ -466,14 +1724,13 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:F7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
@@ -518,19 +1775,19 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>0.91155853849810797</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>0.92465808979605102</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>0.92150203932244301</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <v>0.89707383395541895</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="4">
         <v>0.92805181678916504</v>
       </c>
     </row>
@@ -538,19 +1795,19 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>0.351470877777733</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>0.33107344935587302</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>0.33107344801990701</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>0.57712838860485205</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="4">
         <v>0.33452172584824402</v>
       </c>
     </row>
@@ -558,19 +1815,19 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <v>0.75479836118783294</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>0.94511786517264496</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>0.92293200531085695</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <v>0.972758618634322</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="4">
         <v>0.94931034403285697</v>
       </c>
     </row>
@@ -611,6 +1868,9 @@
       <c r="B9">
         <v>0.38945464573382699</v>
       </c>
+      <c r="C9">
+        <v>0.38618564015268703</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -626,6 +1886,9 @@
       </c>
       <c r="B11">
         <v>0.94797791780502205</v>
+      </c>
+      <c r="C11">
+        <v>0.96153529833013396</v>
       </c>
     </row>
   </sheetData>
@@ -634,9 +1897,10 @@
     <mergeCell ref="A7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add report and update experiments and poster
</commit_message>
<xml_diff>
--- a/doc/final_project_experiments.xlsx
+++ b/doc/final_project_experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hurtja/Documents/Spring2018/CI/CNNFinalProject/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FF755F-FAD8-6144-AFD9-D0D26AE5BB0D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060455A5-0E5C-A04E-B5B3-AF95057DABB4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="19520" xr2:uid="{F6E77F36-42F3-3D4F-B027-6FE579A9FCA2}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" xr2:uid="{F6E77F36-42F3-3D4F-B027-6FE579A9FCA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,19 +107,27 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0%"/>
     </dxf>
@@ -134,14 +142,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1399,18 +1399,18 @@
   <autoFilter ref="A2:F5" xr:uid="{023C54D3-C4E0-0D4C-9E3C-B5C967E3EDB1}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{361F45BA-E1D9-214A-8183-6B8A0E744833}" name="Method"/>
-    <tableColumn id="2" xr3:uid="{EA2E6766-427C-2645-A26B-C347F532F8C8}" name="10" dataDxfId="4" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{A166A588-2222-8343-BC34-F16EE81825E4}" name="20" dataDxfId="3" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{ABB0FA7A-36D2-8F4D-B1BE-764E5E2B471A}" name="30" dataDxfId="2" dataCellStyle="Percent"/>
-    <tableColumn id="5" xr3:uid="{B3AEFE5C-80F8-6847-9162-43DACF35AC3B}" name="40" dataDxfId="1" dataCellStyle="Percent"/>
-    <tableColumn id="6" xr3:uid="{FD2CE875-7E89-324D-B301-C7FFD8CF0FE6}" name="50" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{EA2E6766-427C-2645-A26B-C347F532F8C8}" name="10" dataDxfId="5" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{A166A588-2222-8343-BC34-F16EE81825E4}" name="20" dataDxfId="4" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{ABB0FA7A-36D2-8F4D-B1BE-764E5E2B471A}" name="30" dataDxfId="3" dataCellStyle="Percent"/>
+    <tableColumn id="5" xr3:uid="{B3AEFE5C-80F8-6847-9162-43DACF35AC3B}" name="40" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="6" xr3:uid="{FD2CE875-7E89-324D-B301-C7FFD8CF0FE6}" name="50" dataDxfId="1" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2F99A300-C080-A746-B52B-7ED60B0DC2FD}" name="Table57" displayName="Table57" ref="A8:F11" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2F99A300-C080-A746-B52B-7ED60B0DC2FD}" name="Table57" displayName="Table57" ref="A8:F11" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A8:F11" xr:uid="{0F996CB4-D350-E044-8C03-18674C1CD481}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B8882C41-F743-544E-A47C-3E26F80E0EA2}" name="Method"/>
@@ -1724,7 +1724,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1775,19 +1775,19 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="2">
         <v>0.91155853849810797</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="2">
         <v>0.92465808979605102</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <v>0.92150203932244301</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>0.89707383395541895</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="2">
         <v>0.92805181678916504</v>
       </c>
     </row>
@@ -1795,19 +1795,19 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="2">
         <v>0.351470877777733</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <v>0.33107344935587302</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="2">
         <v>0.33107344801990701</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <v>0.57712838860485205</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <v>0.33452172584824402</v>
       </c>
     </row>
@@ -1815,31 +1815,31 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>0.75479836118783294</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>0.94511786517264496</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <v>0.92293200531085695</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>0.972758618634322</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="2">
         <v>0.94931034403285697</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1871,6 +1871,9 @@
       <c r="C9">
         <v>0.38618564015268703</v>
       </c>
+      <c r="D9">
+        <v>0.35349214571341298</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1879,6 +1882,9 @@
       <c r="B10">
         <v>0.179370914430492</v>
       </c>
+      <c r="C10">
+        <v>0.150590426858218</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1889,6 +1895,9 @@
       </c>
       <c r="C11">
         <v>0.96153529833013396</v>
+      </c>
+      <c r="D11">
+        <v>0.96204305206596397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update experiments and final report
</commit_message>
<xml_diff>
--- a/doc/final_project_experiments.xlsx
+++ b/doc/final_project_experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hurtja/Documents/Spring2018/CI/CNNFinalProject/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12828070-14F9-AD42-9647-DD1992934A89}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79446A6A-7D0E-D043-97BD-E3A53446FB7C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" xr2:uid="{F6E77F36-42F3-3D4F-B027-6FE579A9FCA2}"/>
   </bookViews>
@@ -1724,7 +1724,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1894,6 +1894,9 @@
       <c r="D10">
         <v>0.18620018243242101</v>
       </c>
+      <c r="E10">
+        <v>4.8639206997117899E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1910,6 +1913,9 @@
       </c>
       <c r="E11">
         <v>0.96447150925630099</v>
+      </c>
+      <c r="F11">
+        <v>0.97811823366959705</v>
       </c>
     </row>
   </sheetData>

</xml_diff>